<commit_message>
Updated codes and descriptions
</commit_message>
<xml_diff>
--- a/CEOELA/doe_template.xlsx
+++ b/CEOELA/doe_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q521100\Desktop\Workspace_local\AutoOpti_pipeline\220314_AutoOpti_base\modulesAutoOpti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q521100\Desktop\Workspace_local\0_GitHub_desktop\CEOELA\CEOELA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B00FA4F-E3C4-48A0-830C-5C09CBD13D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA71513-2E74-45C0-B0FB-3396F83899CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="2160" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>design variable</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Response1</t>
-  </si>
-  <si>
-    <t>Output1</t>
   </si>
 </sst>
 </file>
@@ -398,9 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -428,45 +423,27 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -481,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DAE56-BA08-4007-8E1F-FB0202198A17}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,70 +485,25 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>